<commit_message>
finally, order reopening and closure again with inventory recalculation, coding and testing completed!
</commit_message>
<xml_diff>
--- a/soberano/test_cases/order_collect_final_stocks_test_cases.xlsx
+++ b/soberano/test_cases/order_collect_final_stocks_test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="order 6" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="order 1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="order 2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="order 2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="order 6" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="order 1" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">Order 2 specifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp7 is produced in cost center mcc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mp7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw10’s stock before order closure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw10’s stock after order process run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw10’s stock after moving outputs to sales warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mw9 is the sales warehouse (all order outputs end here) mw9’s stock before order closure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mw9’s stock after order closuse</t>
+  </si>
   <si>
     <t xml:space="preserve">Order 6 specifications</t>
   </si>
@@ -30,36 +84,9 @@
     <t xml:space="preserve">mp1 is produced in cost center mcc5 and mp7 in mcc4</t>
   </si>
   <si>
-    <t xml:space="preserve">Inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from warehouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to warehouse</t>
-  </si>
-  <si>
     <t xml:space="preserve">mm4</t>
   </si>
   <si>
-    <t xml:space="preserve">mw10</t>
-  </si>
-  <si>
     <t xml:space="preserve">mm2</t>
   </si>
   <si>
@@ -72,21 +99,6 @@
     <t xml:space="preserve">mp1</t>
   </si>
   <si>
-    <t xml:space="preserve">mp7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mw10’s stock before order closure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mw10’s stock after order process run</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mw10’s stock after moving outputs to sales warehouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qty</t>
-  </si>
-  <si>
     <t xml:space="preserve">mw6’s stock before order closure</t>
   </si>
   <si>
@@ -96,16 +108,7 @@
     <t xml:space="preserve">mw6’s stock after moving outputs to sales warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Mw9 is the sales warehouse (all order outputs end here) mw9’s stock before order closure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mw9’s stock after order closuse</t>
-  </si>
-  <si>
     <t xml:space="preserve">Order 1 specifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order 2 specifications</t>
   </si>
 </sst>
 </file>
@@ -234,21 +237,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.71"/>
   </cols>
   <sheetData>
@@ -297,591 +300,122 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>907184</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <f aca="false">B5*H7</f>
-        <v>4535920</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="0" t="n">
-        <f aca="false">G5*H7</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="n">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <f aca="false">B6*H7</f>
-        <v>10</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">G6*H7</f>
-        <v>5000</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">C5*C15+C6*C16</f>
-        <v>74872687.8777112</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1906.185001</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>959.81808526</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <f aca="false">B14</f>
-        <v>1906.185001</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">C14</f>
-        <v>959.81808526</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="J14" s="0" t="n">
-        <f aca="false">F14</f>
-        <v>1906.185001</v>
+        <f aca="false">F10+B14</f>
+        <v>2</v>
       </c>
       <c r="K14" s="0" t="n">
-        <f aca="false">G14</f>
-        <v>959.81808526</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>2721553000000</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>16.50661561</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <f aca="false">B15-C5</f>
-        <v>2721548464080</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">C15</f>
-        <v>16.50661561</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">F15</f>
-        <v>2721548464080</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">G15</f>
-        <v>16.50661561</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>-26.43339924</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <f aca="false">B16-C6</f>
-        <v>-36.43339924</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">F16</f>
-        <v>-36.43339924</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>456.592</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>10495967.0879729</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <f aca="false">B22+H5</f>
-        <v>461.592</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">B22*C22/F22</f>
-        <v>10382273.9662553</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J22" s="4" t="n">
-        <f aca="false">F22-H5</f>
-        <v>456.592</v>
-      </c>
-      <c r="K22" s="4" t="n">
-        <f aca="false">G22</f>
-        <v>10382273.9662553</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>1000001000</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>155.58763247</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <f aca="false">B23+H6</f>
-        <v>1000006000</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">B23*C23/F23</f>
-        <v>155.586854536505</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="4" t="n">
-        <f aca="false">F23-H6</f>
-        <v>1000001000</v>
-      </c>
-      <c r="K23" s="4" t="n">
-        <f aca="false">G23</f>
-        <v>155.586854536505</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>2207.6226218</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>140955.12386064</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <f aca="false">B24</f>
-        <v>2207.6226218</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">C24</f>
-        <v>140955.12386064</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="4" t="n">
-        <f aca="false">F24</f>
-        <v>2207.6226218</v>
-      </c>
-      <c r="K24" s="4" t="n">
-        <f aca="false">G24</f>
-        <v>140955.12386064</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <f aca="false">H7</f>
-        <v>5</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">J7</f>
-        <v>74872687.8777112</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="4" t="n">
-        <f aca="false">F25-H7</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>999.999</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <f aca="false">B30+H5</f>
-        <v>1004.999</v>
-      </c>
-      <c r="K30" s="0" t="n">
-        <f aca="false">H5*G22/J30</f>
-        <v>51653.1557059028</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <f aca="false">B31+H6</f>
-        <v>5000</v>
-      </c>
-      <c r="K31" s="0" t="n">
-        <f aca="false">(B31*C31+H6*G23)/(B31+H6)</f>
-        <v>155.586854536505</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>7817.4015322</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <f aca="false">B32</f>
-        <v>7817.4015322</v>
-      </c>
-      <c r="K32" s="0" t="n">
-        <f aca="false">C32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <f aca="false">F25</f>
-        <v>5</v>
-      </c>
-      <c r="K33" s="0" t="n">
-        <f aca="false">G25</f>
-        <v>74872687.8777112</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <f aca="false">F18</f>
-        <v>7</v>
-      </c>
-      <c r="K34" s="0" t="n">
-        <f aca="false">G18</f>
+        <f aca="false">(G10*F10+B14*C14)/(B14+F10)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -896,28 +430,28 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,96 +492,96 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>907184</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5*H7</f>
-        <v>907184</v>
+        <v>4535920</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">G5*H7</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6*H7</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">G6*H7</f>
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">C5*C15+C6*C16</f>
-        <v>14974537.5755422</v>
+        <v>74872687.8777112</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>1</v>
@@ -1061,18 +595,18 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -1080,14 +614,14 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>8</v>
@@ -1095,7 +629,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1906.185001</v>
@@ -1104,7 +638,7 @@
         <v>959.81808526</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">B14</f>
@@ -1115,7 +649,7 @@
         <v>959.81808526</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">F14</f>
@@ -1128,31 +662,31 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2721548464080</v>
+        <v>2721553000000</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>16.50661561</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">B15-C5</f>
-        <v>2721547556896</v>
+        <v>2721548464080</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">C15</f>
         <v>16.50661561</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J15" s="0" t="n">
         <f aca="false">F15</f>
-        <v>2721547556896</v>
+        <v>2721548464080</v>
       </c>
       <c r="K15" s="0" t="n">
         <f aca="false">G15</f>
@@ -1161,31 +695,31 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-36.43339924</v>
+        <v>-26.43339924</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">B16-C6</f>
-        <v>-38.43339924</v>
+        <v>-36.43339924</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J16" s="0" t="n">
         <f aca="false">F16</f>
-        <v>-38.43339924</v>
+        <v>-36.43339924</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>0</v>
@@ -1193,7 +727,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -1202,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
@@ -1211,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -1222,7 +756,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -1231,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>7</v>
@@ -1240,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0</v>
@@ -1251,38 +785,38 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>456.592</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>10382273.9662553</v>
+        <v>10495967.0879729</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">B22+H5</f>
-        <v>457.592</v>
+        <v>461.592</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">B22*C22/F22</f>
-        <v>10359585.0338302</v>
+        <v>10382273.9662553</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4" t="n">
         <f aca="false">F22-H5</f>
@@ -1290,32 +824,32 @@
       </c>
       <c r="K22" s="4" t="n">
         <f aca="false">G22</f>
-        <v>10359585.0338302</v>
+        <v>10382273.9662553</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1000001000</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>155.586854536505</v>
+        <v>155.58763247</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">B23+H6</f>
-        <v>1000002000</v>
+        <v>1000006000</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">B23*C23/F23</f>
-        <v>155.586698949962</v>
+        <v>155.586854536505</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J23" s="4" t="n">
         <f aca="false">F23-H6</f>
@@ -1323,12 +857,12 @@
       </c>
       <c r="K23" s="4" t="n">
         <f aca="false">G23</f>
-        <v>155.586698949962</v>
+        <v>155.586854536505</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2207.6226218</v>
@@ -1337,7 +871,7 @@
         <v>140955.12386064</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="false">B24</f>
@@ -1348,7 +882,7 @@
         <v>140955.12386064</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J24" s="4" t="n">
         <f aca="false">F24</f>
@@ -1361,7 +895,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -1370,18 +904,18 @@
         <v>0</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F25" s="0" t="n">
         <f aca="false">H7</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">J7</f>
-        <v>14974537.5755422</v>
+        <v>74872687.8777112</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J25" s="4" t="n">
         <f aca="false">F25-H7</f>
@@ -1393,7 +927,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -1402,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
@@ -1411,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J26" s="4" t="n">
         <v>0</v>
@@ -1422,59 +956,59 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1004.999</v>
+        <v>999.999</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>51093.6447556924</v>
+        <v>0</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J30" s="0" t="n">
         <f aca="false">B30+H5</f>
-        <v>1005.999</v>
+        <v>1004.999</v>
       </c>
       <c r="K30" s="0" t="n">
         <f aca="false">H5*G22/J30</f>
-        <v>10297.8084807542</v>
+        <v>51653.1557059028</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>155.5860766069</v>
+        <v>0</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false">B31+H6</f>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">(B31*C31+H6*G23)/(B31+H6)</f>
-        <v>155.586180330744</v>
+        <v>155.586854536505</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>7817.4015322</v>
@@ -1483,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J32" s="0" t="n">
         <f aca="false">B32</f>
@@ -1496,52 +1030,52 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">F25+B33</f>
         <v>5</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="K33" s="0" t="n">
+        <f aca="false">(F25*G25+B33*C33)/(F25+B33)</f>
         <v>74872687.8777112</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <f aca="false">F25</f>
-        <v>1</v>
-      </c>
-      <c r="K33" s="0" t="n">
-        <f aca="false">G25</f>
-        <v>14974537.5755422</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J34" s="0" t="n">
-        <f aca="false">F18</f>
-        <v>7</v>
+        <f aca="false">F18+B34</f>
+        <v>9</v>
       </c>
       <c r="K34" s="0" t="n">
-        <f aca="false">G18</f>
+        <f aca="false">(B34*C34+F18*G18)/(F18+B34)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1556,28 +1090,28 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,96 +1152,96 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>907184</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5*H7</f>
-        <v>4535920</v>
+        <v>907184</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">G5*H7</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6*H7</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">G6*H7</f>
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">C5*C15+C6*C16</f>
-        <v>74872687.8777112</v>
+        <v>14974537.5755422</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>1</v>
@@ -1721,18 +1255,18 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -1740,14 +1274,14 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>8</v>
@@ -1755,7 +1289,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1906.185001</v>
@@ -1764,7 +1298,7 @@
         <v>959.81808526</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">B14</f>
@@ -1775,7 +1309,7 @@
         <v>959.81808526</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">F14</f>
@@ -1788,31 +1322,31 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2721553000000</v>
+        <v>2721548464080</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>16.50661561</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">B15-C5</f>
-        <v>2721548464080</v>
+        <v>2721547556896</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">C15</f>
         <v>16.50661561</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J15" s="0" t="n">
         <f aca="false">F15</f>
-        <v>2721548464080</v>
+        <v>2721547556896</v>
       </c>
       <c r="K15" s="0" t="n">
         <f aca="false">G15</f>
@@ -1821,31 +1355,31 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-26.43339924</v>
+        <v>-36.43339924</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">B16-C6</f>
-        <v>-36.43339924</v>
+        <v>-38.43339924</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J16" s="0" t="n">
         <f aca="false">F16</f>
-        <v>-36.43339924</v>
+        <v>-38.43339924</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>0</v>
@@ -1853,7 +1387,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -1862,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
@@ -1871,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -1882,7 +1416,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -1891,16 +1425,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0</v>
@@ -1911,38 +1445,38 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>456.592</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>10495967.0879729</v>
+        <v>10382273.9662553</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">B22+H5</f>
-        <v>461.592</v>
+        <v>457.592</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">B22*C22/F22</f>
-        <v>10382273.9662553</v>
+        <v>10359585.0338302</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4" t="n">
         <f aca="false">F22-H5</f>
@@ -1950,32 +1484,32 @@
       </c>
       <c r="K22" s="4" t="n">
         <f aca="false">G22</f>
-        <v>10382273.9662553</v>
+        <v>10359585.0338302</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1000001000</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>155.58763247</v>
+        <v>155.58685454</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">B23+H6</f>
-        <v>1000006000</v>
+        <v>1000002000</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">B23*C23/F23</f>
-        <v>155.586854536505</v>
+        <v>155.586698953457</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J23" s="4" t="n">
         <f aca="false">F23-H6</f>
@@ -1983,12 +1517,12 @@
       </c>
       <c r="K23" s="4" t="n">
         <f aca="false">G23</f>
-        <v>155.586854536505</v>
+        <v>155.586698953457</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2207.6226218</v>
@@ -1997,7 +1531,7 @@
         <v>140955.12386064</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F24" s="0" t="n">
         <f aca="false">B24</f>
@@ -2008,7 +1542,7 @@
         <v>140955.12386064</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J24" s="4" t="n">
         <f aca="false">F24</f>
@@ -2021,7 +1555,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -2030,18 +1564,18 @@
         <v>0</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F25" s="0" t="n">
         <f aca="false">H7</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">J7</f>
-        <v>74872687.8777112</v>
+        <v>14974537.5755422</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J25" s="4" t="n">
         <f aca="false">F25-H7</f>
@@ -2053,7 +1587,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -2062,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
@@ -2071,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J26" s="4" t="n">
         <v>0</v>
@@ -2082,59 +1616,59 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>999.999</v>
+        <v>1004.999</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0</v>
+        <v>51653.1557059028</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J30" s="0" t="n">
         <f aca="false">B30+H5</f>
-        <v>1004.999</v>
+        <v>1005.999</v>
       </c>
       <c r="K30" s="0" t="n">
-        <f aca="false">H5*G22/J30</f>
-        <v>51653.1557059028</v>
+        <f aca="false">(B30*C30+K22)/(B30+H5)</f>
+        <v>61899.6190504233</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0</v>
+        <v>155.586854536505</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false">B31+H6</f>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="K31" s="0" t="n">
         <f aca="false">(B31*C31+H6*G23)/(B31+H6)</f>
-        <v>155.586854536505</v>
+        <v>155.586828605997</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>7817.4015322</v>
@@ -2143,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="J32" s="0" t="n">
         <f aca="false">B32</f>
@@ -2156,45 +1690,45 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0</v>
+        <v>74872687.8777112</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J33" s="0" t="n">
-        <f aca="false">F25</f>
-        <v>5</v>
+        <f aca="false">F25+B33</f>
+        <v>6</v>
       </c>
       <c r="K33" s="0" t="n">
-        <f aca="false">G25</f>
-        <v>74872687.8777112</v>
+        <f aca="false">(G25*F25+C33*B33)/(F25+B33)</f>
+        <v>64889662.8273497</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J34" s="0" t="n">
-        <f aca="false">F18</f>
-        <v>7</v>
+        <f aca="false">F18+B34</f>
+        <v>11</v>
       </c>
       <c r="K34" s="0" t="n">
-        <f aca="false">G18</f>
+        <f aca="false">(G18*F18+B34*C34)/(B34+F18)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>